<commit_message>
Junk values are removed before concat. IP.Abort now tracked as MI
</commit_message>
<xml_diff>
--- a/Utility_Files/Action_definition_Final.xlsx
+++ b/Utility_Files/Action_definition_Final.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sisat\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\GIT\Manual_Intervention\Utility_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="33">
   <si>
     <t>Action_Value</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Val</t>
+  </si>
+  <si>
+    <t>InteractionPar.Abort</t>
   </si>
 </sst>
 </file>
@@ -486,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection sqref="A1:C72"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1286,6 +1289,17 @@
         <v>30</v>
       </c>
     </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>32</v>
+      </c>
+      <c r="C73" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1295,8 +1309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection sqref="A1:B71"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67:B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>